<commit_message>
AUTO FROM work 12.06.2024 11:37:36,07
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -14,9 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="4">
   <si>
-    <t>Hello world</t>
+    <t>Разр. ПО для моб. Платформ ФМЕ ПОИТ3 ЗФПО</t>
+  </si>
+  <si>
+    <t>Резерв</t>
+  </si>
+  <si>
+    <t>СПП (ЗО) 2 курс колония</t>
+  </si>
+  <si>
+    <t>Пусто</t>
   </si>
 </sst>
 </file>
@@ -348,30 +357,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="D4:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="4" spans="4:4">
+      <c r="D4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="E7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="G11" t="s">
-        <v>0</v>
+    <row r="5" spans="4:4">
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:4">
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:4">
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:4">
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="4:4">
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="4:4">
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="4:4">
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4">
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4">
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4">
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4">
+      <c r="D46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4">
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4">
+      <c r="D48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4">
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4">
+      <c r="D50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4">
+      <c r="D54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4">
+      <c r="D55" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4">
+      <c r="D56" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4">
+      <c r="D57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4">
+      <c r="D58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4">
+      <c r="D59" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>